<commit_message>
SC updated to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_SC.xlsx
+++ b/curation/draft/collection/collection_specialization_SC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D850ED1F-12BE-CA47-A656-681070D79B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E04AF3-5A87-CA48-B84F-5787B03D2DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <t>package_date</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Number of Years of Education (Denormalized)</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,14 +626,14 @@
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="11" max="11" width="40.1640625" customWidth="1"/>
-    <col min="14" max="14" width="31" customWidth="1"/>
-    <col min="18" max="18" width="52" customWidth="1"/>
-    <col min="30" max="30" width="19.33203125" customWidth="1"/>
-    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="40.1640625" customWidth="1"/>
+    <col min="15" max="15" width="31" customWidth="1"/>
+    <col min="19" max="19" width="52" customWidth="1"/>
+    <col min="31" max="31" width="19.33203125" customWidth="1"/>
+    <col min="34" max="34" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,82 +665,85 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -759,50 +765,50 @@
       <c r="I2" t="s">
         <v>71</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>360</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>74</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>41</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>42</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>43</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>100</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>44</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>35</v>
       </c>
@@ -824,47 +830,47 @@
       <c r="I3" t="s">
         <v>71</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>360</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>74</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>38</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>45</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>46</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>47</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>38</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>43</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>100</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>48</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>50</v>
       </c>
@@ -886,50 +892,50 @@
       <c r="I4" t="s">
         <v>71</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>360</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>75</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>51</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>52</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>53</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>40</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>41</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>1</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>42</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>43</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>100</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>44</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>40</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -951,50 +957,50 @@
       <c r="I5" t="s">
         <v>71</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>360</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>75</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>51</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>52</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>54</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>46</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>55</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>52</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>2</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>67</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>4</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>50</v>
       </c>
@@ -1016,55 +1022,55 @@
       <c r="I6" t="s">
         <v>71</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>360</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>75</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>51</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>52</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>58</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>59</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>60</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>3</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>43</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>50</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>61</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>62</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>64</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>63</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>65</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added derivation columns (blank) - SC
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_SC.xlsx
+++ b/curation/draft/collection/collection_specialization_SC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E04AF3-5A87-CA48-B84F-5787B03D2DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69D307E-7198-5549-94EF-70238F1AFD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>package_date</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -615,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -629,11 +635,11 @@
     <col min="12" max="12" width="40.1640625" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
     <col min="19" max="19" width="52" customWidth="1"/>
-    <col min="31" max="31" width="19.33203125" customWidth="1"/>
-    <col min="34" max="34" width="15.33203125" customWidth="1"/>
+    <col min="33" max="33" width="19.33203125" customWidth="1"/>
+    <col min="36" max="36" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,40 +716,46 @@
         <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -798,17 +810,17 @@
       <c r="W2">
         <v>100</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>35</v>
       </c>
@@ -863,14 +875,14 @@
       <c r="W3">
         <v>100</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AI3" t="s">
         <v>48</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>50</v>
       </c>
@@ -925,17 +937,17 @@
       <c r="W4">
         <v>100</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>44</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AI4" t="s">
         <v>40</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AJ4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -993,14 +1005,14 @@
       <c r="X5">
         <v>1</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AI5" t="s">
         <v>48</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AJ5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>50</v>
       </c>
@@ -1055,22 +1067,22 @@
       <c r="W6">
         <v>50</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
         <v>61</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AC6" t="s">
         <v>62</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>64</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>63</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AI6" t="s">
         <v>65</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AJ6" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>